<commit_message>
updated medicine list date and spreadsheet content
</commit_message>
<xml_diff>
--- a/app/data/medications.xlsx
+++ b/app/data/medications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/hrt-ppc/app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CHCHI/Documents/Prototypes/HRT-PPC/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DE936F-2910-514A-9A7A-D4A5C5F30304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D26B6C3-B301-014E-9F5E-B4615DFE7EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="13940" xr2:uid="{7B130118-B2A6-1E4F-852E-77291D9083D4}"/>
+    <workbookView xWindow="80" yWindow="760" windowWidth="25440" windowHeight="13940" xr2:uid="{7B130118-B2A6-1E4F-852E-77291D9083D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
   <si>
     <t>Brand name</t>
   </si>
@@ -215,9 +215,6 @@
     <t>Levonorgestrel 20micrograms/24hours intrauterine device</t>
   </si>
   <si>
-    <t>Non-branded products</t>
-  </si>
-  <si>
     <t>Estriol 500microgram pessaries</t>
   </si>
   <si>
@@ -236,30 +233,12 @@
     <t>Estradiol 0.06% gel (750microgram per actuation)</t>
   </si>
   <si>
-    <t>Ovestin</t>
-  </si>
-  <si>
-    <t>Estriol 1mg/g vaginal cream</t>
-  </si>
-  <si>
-    <t>Premarin</t>
-  </si>
-  <si>
     <t>Conjugated oestrogens 300microgram tablets</t>
   </si>
   <si>
     <t>Conjugated oestrogens 625microgram tablets</t>
   </si>
   <si>
-    <t>Conjugated oestrogens 1.25mg tablets</t>
-  </si>
-  <si>
-    <t>Premique low dose</t>
-  </si>
-  <si>
-    <t>Conjugated oestrogens 300microgram / Medroxyprogesterone 1.5mg modified-release tablets</t>
-  </si>
-  <si>
     <t>Progynova</t>
   </si>
   <si>
@@ -333,6 +312,24 @@
   </si>
   <si>
     <t>Prasterone</t>
+  </si>
+  <si>
+    <t>Non-branded products not listed elsewhere in the table</t>
+  </si>
+  <si>
+    <t>Conjugated oestrogens 1.25microgram tablets</t>
+  </si>
+  <si>
+    <t>Estriol 0.01% vaginal cream</t>
+  </si>
+  <si>
+    <t>Medroxyprogesterone 1.5mg modified-release tablets</t>
+  </si>
+  <si>
+    <t>Nalvee</t>
+  </si>
+  <si>
+    <t>Dydrogesterone 10mg tablets</t>
   </si>
 </sst>
 </file>
@@ -718,20 +715,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B65CFC5-C783-504F-9132-74AA62817378}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="29.83203125" customWidth="1"/>
+    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="85" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
     <col min="5" max="5" width="49.6640625" customWidth="1"/>
     <col min="6" max="6" width="48.5" customWidth="1"/>
     <col min="7" max="7" width="57.6640625" customWidth="1"/>
+    <col min="8" max="8" width="37.6640625" customWidth="1"/>
+    <col min="9" max="9" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -739,18 +739,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -761,7 +761,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -783,7 +783,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -794,7 +794,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -808,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -828,7 +828,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -851,7 +851,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -862,7 +862,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -882,7 +882,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
@@ -912,7 +912,7 @@
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
         <v>30</v>
@@ -926,7 +926,7 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -943,71 +943,71 @@
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1021,62 +1021,62 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -1084,174 +1084,161 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" t="s">
         <v>59</v>
       </c>
-      <c r="B29" t="s">
+      <c r="G30" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" t="s">
         <v>94</v>
       </c>
-      <c r="C29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="I30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="C31" t="s">
         <v>62</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
         <v>64</v>
       </c>
-      <c r="B31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>69</v>
       </c>
-      <c r="D33" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>70</v>
       </c>
-      <c r="E33" t="s">
+      <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" t="s">
         <v>72</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>74</v>
       </c>
-      <c r="B35" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>75</v>
       </c>
-      <c r="D35" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="C37" t="s">
         <v>77</v>
       </c>
-      <c r="B36" t="s">
-        <v>97</v>
-      </c>
-      <c r="C36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>78</v>
       </c>
-      <c r="B37" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>79</v>
       </c>
-      <c r="D37" t="s">
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>81</v>
       </c>
-      <c r="C38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>86</v>
-      </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" t="s">
-        <v>93</v>
-      </c>
-      <c r="C42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" t="s">
         <v>16</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D41" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated medicine list for Nov 1 release
</commit_message>
<xml_diff>
--- a/app/data/medications.xlsx
+++ b/app/data/medications.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CHCHI/Documents/Prototypes/HRT-PPC/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D26B6C3-B301-014E-9F5E-B4615DFE7EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEC79A6-07B8-694B-B6B7-A2E54F148240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="760" windowWidth="25440" windowHeight="13940" xr2:uid="{7B130118-B2A6-1E4F-852E-77291D9083D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="103">
   <si>
     <t>Brand name</t>
   </si>
@@ -330,6 +330,21 @@
   </si>
   <si>
     <t>Dydrogesterone 10mg tablets</t>
+  </si>
+  <si>
+    <t>Estradot Conti</t>
+  </si>
+  <si>
+    <t>Estradiol 30micrograms/24hours / Norethisterone 95micrograms/24hours transdermal patches</t>
+  </si>
+  <si>
+    <t>Estradiol 40micrograms/24hours / Norethisterone 130micrograms/24hours transdermal patches</t>
+  </si>
+  <si>
+    <t>Ovesse</t>
+  </si>
+  <si>
+    <t>Estriol 1mg/g vaginal cream with applicator</t>
   </si>
 </sst>
 </file>
@@ -715,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B65CFC5-C783-504F-9132-74AA62817378}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,7 +741,7 @@
     <col min="1" max="1" width="47.6640625" customWidth="1"/>
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="85" customWidth="1"/>
-    <col min="4" max="4" width="52" customWidth="1"/>
+    <col min="4" max="4" width="81.6640625" customWidth="1"/>
     <col min="5" max="5" width="49.6640625" customWidth="1"/>
     <col min="6" max="6" width="48.5" customWidth="1"/>
     <col min="7" max="7" width="57.6640625" customWidth="1"/>
@@ -848,397 +863,422 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
         <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
         <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
         <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
         <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
         <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" t="s">
-        <v>59</v>
-      </c>
-      <c r="G30" t="s">
-        <v>60</v>
-      </c>
-      <c r="H30" t="s">
-        <v>94</v>
-      </c>
-      <c r="I30" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
         <v>90</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>19</v>
+      </c>
+      <c r="D36" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>81</v>
       </c>
-      <c r="B41" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" t="s">
         <v>16</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D43" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>